<commit_message>
test data changes, footer, inactive details
</commit_message>
<xml_diff>
--- a/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
+++ b/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992A2706-7CC9-4311-AF8E-E64DC79520E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEC791A-B5A9-45CF-BB37-FDEE84C824D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="10837" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="10837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="FooterLinks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
@@ -778,7 +778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709CE98B-E627-491B-8C47-135D5895C63F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test data changes, new test link
</commit_message>
<xml_diff>
--- a/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
+++ b/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2634236-0AB8-42AE-8F55-A952D6A450DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6ACECC-C19B-44F0-97CC-A97A23BC3DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="10837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>DataSet</t>
   </si>
@@ -63,6 +63,57 @@
   </si>
   <si>
     <t>8186886443</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>FPGNCW000005A</t>
+  </si>
+  <si>
+    <t>bJfH83IKu8</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>vinjamuriajay@flypigeon.com</t>
+  </si>
+  <si>
+    <t>QueryID</t>
+  </si>
+  <si>
+    <t>FPGNCALL000001</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>07/03/2023</t>
+  </si>
+  <si>
+    <t>26/03/2023</t>
+  </si>
+  <si>
+    <t>8008554070</t>
+  </si>
+  <si>
+    <t>Inactive details</t>
+  </si>
+  <si>
+    <t>FPGNR8000007A</t>
   </si>
 </sst>
 </file>
@@ -130,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -139,6 +190,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,96 +473,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="2" max="5" width="23.1796875" customWidth="1"/>
+    <col min="6" max="6" width="100.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" s="2"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D12" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="4"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="4"/>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="6"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="4"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H22" s="6"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="I23" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{3A24BFA4-45E0-4C02-9649-896BEBF2B70E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -518,12 +635,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
itinerary and passenger details
</commit_message>
<xml_diff>
--- a/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
+++ b/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CDEB3A-57C0-4DA6-9390-F0F71FC1CB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6834FD82-4968-4CF3-9307-41D14644B5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="10837" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>DataSet</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>Agent</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly </t>
+  </si>
+  <si>
+    <t>Pegion</t>
   </si>
 </sst>
 </file>
@@ -563,32 +578,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="3" width="23.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
-    <col min="7" max="10" width="9.6328125" customWidth="1"/>
-    <col min="11" max="11" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.6328125" customWidth="1"/>
-    <col min="15" max="15" width="100.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.81640625" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1796875" customWidth="1"/>
-    <col min="20" max="20" width="10.6328125" customWidth="1"/>
-    <col min="21" max="21" width="10.453125" customWidth="1"/>
-    <col min="22" max="22" width="20.81640625" customWidth="1"/>
-    <col min="23" max="23" width="23.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="10" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.6640625" customWidth="1"/>
+    <col min="15" max="15" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.77734375" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.21875" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
+    <col min="21" max="21" width="10.44140625" customWidth="1"/>
+    <col min="22" max="22" width="20.77734375" customWidth="1"/>
+    <col min="23" max="23" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -678,7 +693,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -701,7 +716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -734,7 +749,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -743,7 +758,7 @@
       </c>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -776,7 +791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -803,23 +818,23 @@
       </c>
       <c r="R7" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q12" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="Q14" s="2"/>
     </row>
-    <row r="18" spans="17:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="17:18" x14ac:dyDescent="0.3">
       <c r="R18" s="4"/>
     </row>
-    <row r="20" spans="17:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="17:18" x14ac:dyDescent="0.3">
       <c r="R20" s="4"/>
     </row>
-    <row r="22" spans="17:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="17:18" x14ac:dyDescent="0.3">
       <c r="Q22" s="6"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="17:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="17:18" x14ac:dyDescent="0.3">
       <c r="R23" s="4"/>
     </row>
   </sheetData>
@@ -841,9 +856,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,7 +866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -866,15 +881,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B74D610A-0754-471F-9B9F-9DF81FB0FED4}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,25 +916,28 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -923,24 +948,40 @@
         <v>35</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="I3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
       <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4C74CBF8-85D8-4160-8560-682A35AEC5FB}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{670D28E5-98B8-4879-BF8E-35DA6391C1F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
helper test data changes
</commit_message>
<xml_diff>
--- a/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
+++ b/Gold_Fly/src/test/resources/TestData/FlyPegion/FlyPegionTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896D03F4-D3AB-440F-BC34-B5850EBE35BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F88E208-5A9D-4A78-953D-5093630F99D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="10837" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>DataSet</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Air Booking list</t>
+  </si>
+  <si>
+    <t>bus booking list</t>
   </si>
 </sst>
 </file>
@@ -604,31 +607,31 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9.6640625" customWidth="1"/>
-    <col min="15" max="15" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.77734375" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.21875" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" customWidth="1"/>
-    <col min="22" max="22" width="20.77734375" customWidth="1"/>
-    <col min="23" max="23" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="2" max="3" width="23.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="7" max="10" width="9.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.6328125" customWidth="1"/>
+    <col min="15" max="15" width="100.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1796875" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" customWidth="1"/>
+    <col min="22" max="22" width="20.81640625" customWidth="1"/>
+    <col min="23" max="23" width="23.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +702,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -718,7 +721,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -741,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -774,7 +777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -783,7 +786,7 @@
       </c>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -816,7 +819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -843,23 +846,23 @@
       </c>
       <c r="R7" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="Q12" s="5"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="Q14" s="2"/>
     </row>
-    <row r="18" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:18" x14ac:dyDescent="0.35">
       <c r="R18" s="4"/>
     </row>
-    <row r="20" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="17:18" x14ac:dyDescent="0.35">
       <c r="R20" s="4"/>
     </row>
-    <row r="22" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="17:18" x14ac:dyDescent="0.35">
       <c r="Q22" s="6"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="17:18" x14ac:dyDescent="0.35">
       <c r="R23" s="4"/>
     </row>
   </sheetData>
@@ -881,9 +884,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -912,16 +915,16 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -974,7 +977,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -986,7 +989,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1014,20 +1017,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C73008-F68E-4194-BF56-080D36766BB8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1046,11 @@
       <c r="E1" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>65</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1066,12 +1072,20 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>